<commit_message>
3 dpi phage count data for plate experiment 2
</commit_message>
<xml_diff>
--- a/Plate_bn_exp_2/data/plate2_counts.xlsx
+++ b/Plate_bn_exp_2/data/plate2_counts.xlsx
@@ -391,8 +391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1771,8 +1771,8 @@
       <c r="C98" t="s">
         <v>6</v>
       </c>
-      <c r="D98">
-        <v>120000000</v>
+      <c r="D98" s="1">
+        <v>120000</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -1785,8 +1785,8 @@
       <c r="C99" t="s">
         <v>6</v>
       </c>
-      <c r="D99">
-        <v>320000000</v>
+      <c r="D99" s="1">
+        <v>320000</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -1799,8 +1799,8 @@
       <c r="C100" t="s">
         <v>6</v>
       </c>
-      <c r="D100">
-        <v>2000000000</v>
+      <c r="D100" s="1">
+        <v>2000000</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -1813,8 +1813,8 @@
       <c r="C101" t="s">
         <v>6</v>
       </c>
-      <c r="D101">
-        <v>180000000</v>
+      <c r="D101" s="1">
+        <v>180000</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -1827,8 +1827,8 @@
       <c r="C102" t="s">
         <v>6</v>
       </c>
-      <c r="D102">
-        <v>160000000</v>
+      <c r="D102" s="1">
+        <v>160000</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -1841,8 +1841,8 @@
       <c r="C103" t="s">
         <v>6</v>
       </c>
-      <c r="D103">
-        <v>460000000</v>
+      <c r="D103" s="1">
+        <v>460000</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -1939,7 +1939,9 @@
       <c r="C110" t="s">
         <v>7</v>
       </c>
-      <c r="D110" s="1"/>
+      <c r="D110" s="1">
+        <v>5800000000</v>
+      </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="4">
@@ -1951,7 +1953,9 @@
       <c r="C111" t="s">
         <v>7</v>
       </c>
-      <c r="D111" s="1"/>
+      <c r="D111" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
@@ -1963,7 +1967,9 @@
       <c r="C112" t="s">
         <v>7</v>
       </c>
-      <c r="D112" s="1"/>
+      <c r="D112" s="1">
+        <v>3.6E-9</v>
+      </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
@@ -1975,7 +1981,9 @@
       <c r="C113" t="s">
         <v>7</v>
       </c>
-      <c r="D113" s="1"/>
+      <c r="D113" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="4">
@@ -1987,7 +1995,9 @@
       <c r="C114" t="s">
         <v>7</v>
       </c>
-      <c r="D114" s="1"/>
+      <c r="D114" s="1">
+        <v>46000000000</v>
+      </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="4">
@@ -1999,7 +2009,9 @@
       <c r="C115" t="s">
         <v>7</v>
       </c>
-      <c r="D115" s="1"/>
+      <c r="D115" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="4">
@@ -2011,7 +2023,9 @@
       <c r="C116" t="s">
         <v>7</v>
       </c>
-      <c r="D116" s="1"/>
+      <c r="D116" s="1">
+        <v>700000000</v>
+      </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="4">
@@ -2023,7 +2037,9 @@
       <c r="C117" t="s">
         <v>7</v>
       </c>
-      <c r="D117" s="1"/>
+      <c r="D117" s="1">
+        <v>1000000000000</v>
+      </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="4">
@@ -2035,7 +2051,9 @@
       <c r="C118" t="s">
         <v>7</v>
       </c>
-      <c r="D118" s="1"/>
+      <c r="D118" s="1">
+        <v>26000000000</v>
+      </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="4">
@@ -2047,7 +2065,9 @@
       <c r="C119" t="s">
         <v>7</v>
       </c>
-      <c r="D119" s="1"/>
+      <c r="D119" s="1">
+        <v>3400000000</v>
+      </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="4">
@@ -2059,7 +2079,9 @@
       <c r="C120" t="s">
         <v>7</v>
       </c>
-      <c r="D120" s="1"/>
+      <c r="D120" s="1">
+        <v>18000000000</v>
+      </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="4">
@@ -2071,7 +2093,9 @@
       <c r="C121" t="s">
         <v>7</v>
       </c>
-      <c r="D121" s="1"/>
+      <c r="D121" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="4">
@@ -2083,7 +2107,9 @@
       <c r="C122" t="s">
         <v>7</v>
       </c>
-      <c r="D122" s="1"/>
+      <c r="D122" s="1">
+        <v>30000000</v>
+      </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
@@ -2095,7 +2121,9 @@
       <c r="C123" t="s">
         <v>7</v>
       </c>
-      <c r="D123" s="1"/>
+      <c r="D123" s="1">
+        <v>2600000000</v>
+      </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
@@ -2107,7 +2135,9 @@
       <c r="C124" t="s">
         <v>7</v>
       </c>
-      <c r="D124" s="1"/>
+      <c r="D124" s="1">
+        <v>520000000000</v>
+      </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
@@ -2119,7 +2149,9 @@
       <c r="C125" t="s">
         <v>7</v>
       </c>
-      <c r="D125" s="1"/>
+      <c r="D125" s="1">
+        <v>1200000000000</v>
+      </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="4">
@@ -2131,7 +2163,9 @@
       <c r="C126" t="s">
         <v>7</v>
       </c>
-      <c r="D126" s="1"/>
+      <c r="D126" s="1">
+        <v>400</v>
+      </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="4">
@@ -2143,7 +2177,9 @@
       <c r="C127" t="s">
         <v>7</v>
       </c>
-      <c r="D127" s="1"/>
+      <c r="D127" s="1">
+        <v>26000000000</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="4">
@@ -2155,7 +2191,9 @@
       <c r="C128" t="s">
         <v>7</v>
       </c>
-      <c r="D128" s="1"/>
+      <c r="D128" s="1">
+        <v>260000</v>
+      </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="4">
@@ -2167,7 +2205,9 @@
       <c r="C129" t="s">
         <v>7</v>
       </c>
-      <c r="D129" s="1"/>
+      <c r="D129" s="1">
+        <v>3200000</v>
+      </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="4">
@@ -2179,7 +2219,9 @@
       <c r="C130" t="s">
         <v>7</v>
       </c>
-      <c r="D130" s="1"/>
+      <c r="D130" s="1">
+        <v>1000</v>
+      </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="4">
@@ -2191,7 +2233,9 @@
       <c r="C131" t="s">
         <v>7</v>
       </c>
-      <c r="D131" s="1"/>
+      <c r="D131" s="1">
+        <v>3200000000</v>
+      </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="4">
@@ -2203,7 +2247,9 @@
       <c r="C132" t="s">
         <v>7</v>
       </c>
-      <c r="D132" s="1"/>
+      <c r="D132" s="1">
+        <v>52000000</v>
+      </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="4">
@@ -2215,7 +2261,9 @@
       <c r="C133" t="s">
         <v>7</v>
       </c>
-      <c r="D133" s="1"/>
+      <c r="D133" s="1">
+        <v>38000000</v>
+      </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="4">
@@ -2227,7 +2275,7 @@
       <c r="C134" t="s">
         <v>7</v>
       </c>
-      <c r="D134">
+      <c r="D134" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2241,8 +2289,8 @@
       <c r="C135" t="s">
         <v>7</v>
       </c>
-      <c r="D135">
-        <v>14000</v>
+      <c r="D135" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -2255,8 +2303,8 @@
       <c r="C136" t="s">
         <v>7</v>
       </c>
-      <c r="D136">
-        <v>2000</v>
+      <c r="D136" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -2269,8 +2317,8 @@
       <c r="C137" t="s">
         <v>7</v>
       </c>
-      <c r="D137">
-        <v>1200000</v>
+      <c r="D137" s="1">
+        <v>1200</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -2283,8 +2331,8 @@
       <c r="C138" t="s">
         <v>7</v>
       </c>
-      <c r="D138">
-        <v>360000</v>
+      <c r="D138" s="1">
+        <v>360</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -2297,8 +2345,8 @@
       <c r="C139" t="s">
         <v>7</v>
       </c>
-      <c r="D139">
-        <v>4000</v>
+      <c r="D139" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -2311,7 +2359,9 @@
       <c r="C140" t="s">
         <v>7</v>
       </c>
-      <c r="D140" s="1"/>
+      <c r="D140" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="4">
@@ -2323,7 +2373,9 @@
       <c r="C141" t="s">
         <v>7</v>
       </c>
-      <c r="D141" s="1"/>
+      <c r="D141" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="4">
@@ -2335,7 +2387,9 @@
       <c r="C142" t="s">
         <v>7</v>
       </c>
-      <c r="D142" s="1"/>
+      <c r="D142" s="1">
+        <v>600</v>
+      </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="4">
@@ -2347,7 +2401,9 @@
       <c r="C143" t="s">
         <v>7</v>
       </c>
-      <c r="D143" s="1"/>
+      <c r="D143" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="4">
@@ -2359,7 +2415,9 @@
       <c r="C144" t="s">
         <v>7</v>
       </c>
-      <c r="D144" s="1"/>
+      <c r="D144" s="1">
+        <v>200</v>
+      </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="4">
@@ -2371,7 +2429,9 @@
       <c r="C145" t="s">
         <v>7</v>
       </c>
-      <c r="D145" s="1"/>
+      <c r="D145" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="4">
@@ -2694,7 +2754,7 @@
       <c r="C170" t="s">
         <v>8</v>
       </c>
-      <c r="D170">
+      <c r="D170" s="1">
         <v>0</v>
       </c>
       <c r="E170" s="1"/>
@@ -2709,7 +2769,7 @@
       <c r="C171" t="s">
         <v>8</v>
       </c>
-      <c r="D171">
+      <c r="D171" s="1">
         <v>0</v>
       </c>
       <c r="E171" s="1"/>
@@ -2724,7 +2784,7 @@
       <c r="C172" t="s">
         <v>8</v>
       </c>
-      <c r="D172">
+      <c r="D172" s="1">
         <v>0</v>
       </c>
       <c r="E172" s="1"/>
@@ -2739,7 +2799,7 @@
       <c r="C173" t="s">
         <v>8</v>
       </c>
-      <c r="D173">
+      <c r="D173" s="1">
         <v>0</v>
       </c>
       <c r="E173" s="1"/>
@@ -2754,7 +2814,7 @@
       <c r="C174" t="s">
         <v>8</v>
       </c>
-      <c r="D174">
+      <c r="D174" s="1">
         <v>0</v>
       </c>
       <c r="E174" s="1"/>
@@ -2769,7 +2829,7 @@
       <c r="C175" t="s">
         <v>8</v>
       </c>
-      <c r="D175">
+      <c r="D175" s="1">
         <v>0</v>
       </c>
       <c r="E175" s="1"/>
@@ -3151,7 +3211,7 @@
       <c r="C206" t="s">
         <v>9</v>
       </c>
-      <c r="D206">
+      <c r="D206" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3165,7 +3225,7 @@
       <c r="C207" t="s">
         <v>9</v>
       </c>
-      <c r="D207">
+      <c r="D207" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3179,7 +3239,7 @@
       <c r="C208" t="s">
         <v>9</v>
       </c>
-      <c r="D208">
+      <c r="D208" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3193,7 +3253,7 @@
       <c r="C209" t="s">
         <v>9</v>
       </c>
-      <c r="D209">
+      <c r="D209" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3207,7 +3267,7 @@
       <c r="C210" t="s">
         <v>9</v>
       </c>
-      <c r="D210">
+      <c r="D210" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3221,7 +3281,7 @@
       <c r="C211" t="s">
         <v>9</v>
       </c>
-      <c r="D211">
+      <c r="D211" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>